<commit_message>
matrice d'agregation des pays pour 3 blocs
</commit_message>
<xml_diff>
--- a/List_Countries.xlsx
+++ b/List_Countries.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ubuntu\M2_EEET\Optimisation_incertain\Optim_trade_policy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ancel\Desktop\M2_EEET\Optim_trade_policy-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FD9F97-8C0B-41AA-9BEB-13860EF0FA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10812" yWindow="1800" windowWidth="11664" windowHeight="8964" xr2:uid="{C5523EA0-181B-4662-8B4D-AA3B5E79CB20}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7900"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="141">
   <si>
     <t>111 303 343 689</t>
   </si>
@@ -448,12 +447,21 @@
   </si>
   <si>
     <t>Iceland</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>Asia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -517,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -532,6 +540,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,20 +856,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEBF7E4F-40F1-46E1-9C06-E2BCAE24385B}">
-  <dimension ref="A1:D47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="5"/>
+    <col min="2" max="2" width="17.90625" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>134</v>
       </c>
@@ -868,8 +879,17 @@
       <c r="C1" s="5" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>49</v>
       </c>
@@ -879,9 +899,17 @@
       <c r="C2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>50</v>
       </c>
@@ -891,8 +919,17 @@
       <c r="C3" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
@@ -902,8 +939,17 @@
       <c r="C4" s="4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -913,8 +959,17 @@
       <c r="C5" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
@@ -924,8 +979,17 @@
       <c r="C6" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
@@ -935,8 +999,17 @@
       <c r="C7" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
@@ -946,8 +1019,17 @@
       <c r="C8" s="4" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
@@ -957,8 +1039,17 @@
       <c r="C9" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
@@ -968,8 +1059,17 @@
       <c r="C10" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -979,8 +1079,17 @@
       <c r="C11" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>59</v>
       </c>
@@ -990,8 +1099,14 @@
       <c r="C12" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>60</v>
       </c>
@@ -1001,8 +1116,14 @@
       <c r="C13" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
@@ -1012,8 +1133,14 @@
       <c r="C14" s="4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>62</v>
       </c>
@@ -1023,8 +1150,11 @@
       <c r="C15" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>63</v>
       </c>
@@ -1034,8 +1164,11 @@
       <c r="C16" s="4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>64</v>
       </c>
@@ -1045,8 +1178,11 @@
       <c r="C17" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1056,8 +1192,11 @@
       <c r="C18" s="4" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>65</v>
       </c>
@@ -1067,8 +1206,11 @@
       <c r="C19" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>66</v>
       </c>
@@ -1078,8 +1220,11 @@
       <c r="C20" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>67</v>
       </c>
@@ -1089,8 +1234,11 @@
       <c r="C21" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
@@ -1100,8 +1248,11 @@
       <c r="C22" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -1111,8 +1262,11 @@
       <c r="C23" s="4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
@@ -1123,7 +1277,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1134,7 +1288,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>71</v>
       </c>
@@ -1145,7 +1299,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -1156,7 +1310,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1167,7 +1321,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>73</v>
       </c>
@@ -1178,7 +1332,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>74</v>
       </c>
@@ -1189,7 +1343,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>75</v>
       </c>
@@ -1200,7 +1354,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>76</v>
       </c>
@@ -1211,7 +1365,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>77</v>
       </c>
@@ -1222,7 +1376,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>78</v>
       </c>
@@ -1233,7 +1387,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>79</v>
       </c>
@@ -1244,7 +1398,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>80</v>
       </c>
@@ -1255,7 +1409,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
@@ -1266,7 +1420,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>82</v>
       </c>
@@ -1277,7 +1431,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>83</v>
       </c>
@@ -1288,7 +1442,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>84</v>
       </c>
@@ -1299,7 +1453,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1310,7 +1464,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>86</v>
       </c>
@@ -1321,7 +1475,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
         <v>87</v>
       </c>
@@ -1332,7 +1486,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>88</v>
       </c>
@@ -1343,7 +1497,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -1354,7 +1508,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
         <v>137</v>
       </c>
@@ -1365,7 +1519,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="1"/>
       <c r="C47" s="4"/>

</xml_diff>